<commit_message>
Added the If condition to handle setup change
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/POData_AutomationOrg.xlsx
+++ b/templates/AutomationOrg/POData_AutomationOrg.xlsx
@@ -442,7 +442,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="70" x14ac:knownFonts="1">
+  <fonts count="150" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -479,6 +479,486 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -885,7 +1365,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="73">
     <border>
       <left/>
       <right/>
@@ -989,11 +1469,131 @@
     <border>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="154">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
@@ -1070,8 +1670,88 @@
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="30" fillId="0" fontId="65" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="66" numFmtId="164" xfId="0"/>
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="31" fillId="0" fontId="67" numFmtId="49" xfId="0"/>
-    <xf numFmtId="164" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="69" fillId="0" borderId="32" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="68" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="32" fillId="0" fontId="69" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="70" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="33" fillId="0" fontId="71" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="72" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="34" fillId="0" fontId="73" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="74" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="35" fillId="0" fontId="75" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="76" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="36" fillId="0" fontId="77" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="78" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="37" fillId="0" fontId="79" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="80" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="38" fillId="0" fontId="81" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="82" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="39" fillId="0" fontId="83" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="84" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="40" fillId="0" fontId="85" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="86" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="41" fillId="0" fontId="87" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="88" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="42" fillId="0" fontId="89" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="90" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="43" fillId="0" fontId="91" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="92" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="44" fillId="0" fontId="93" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="94" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="45" fillId="0" fontId="95" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="96" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="46" fillId="0" fontId="97" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="98" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="47" fillId="0" fontId="99" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="100" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="48" fillId="0" fontId="101" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="102" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="49" fillId="0" fontId="103" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="104" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="50" fillId="0" fontId="105" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="106" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="51" fillId="0" fontId="107" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="108" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="52" fillId="0" fontId="109" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="110" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="53" fillId="0" fontId="111" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="112" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="54" fillId="0" fontId="113" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="114" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="55" fillId="0" fontId="115" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="116" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="56" fillId="0" fontId="117" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="118" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="57" fillId="0" fontId="119" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="120" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="58" fillId="0" fontId="121" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="122" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="59" fillId="0" fontId="123" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="124" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="60" fillId="0" fontId="125" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="126" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="61" fillId="0" fontId="127" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="128" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="62" fillId="0" fontId="129" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="130" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="63" fillId="0" fontId="131" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="132" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="64" fillId="0" fontId="133" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="134" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="65" fillId="0" fontId="135" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="136" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="66" fillId="0" fontId="137" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="138" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="67" fillId="0" fontId="139" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="140" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="68" fillId="0" fontId="141" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="142" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="69" fillId="0" fontId="143" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="144" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="70" fillId="0" fontId="145" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="146" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="71" fillId="0" fontId="147" numFmtId="49" xfId="0"/>
+    <xf numFmtId="164" fontId="148" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="149" fillId="0" borderId="72" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>

</xml_diff>

<commit_message>
Purchase Req TC update
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/POData_AutomationOrg.xlsx
+++ b/templates/AutomationOrg/POData_AutomationOrg.xlsx
@@ -442,7 +442,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="150" x14ac:knownFonts="1">
+  <fonts count="318" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -479,6 +479,1014 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -1365,7 +2373,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="73">
+  <borders count="157">
     <border>
       <left/>
       <right/>
@@ -1589,11 +2597,263 @@
     <border>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="322">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
@@ -1750,8 +3010,176 @@
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="70" fillId="0" fontId="145" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="146" numFmtId="164" xfId="0"/>
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="71" fillId="0" fontId="147" numFmtId="49" xfId="0"/>
-    <xf numFmtId="164" fontId="148" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="149" fillId="0" borderId="72" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="148" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="72" fillId="0" fontId="149" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="150" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="73" fillId="0" fontId="151" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="152" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="74" fillId="0" fontId="153" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="154" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="75" fillId="0" fontId="155" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="156" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="76" fillId="0" fontId="157" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="158" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="77" fillId="0" fontId="159" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="160" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="78" fillId="0" fontId="161" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="162" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="79" fillId="0" fontId="163" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="164" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="80" fillId="0" fontId="165" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="166" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="81" fillId="0" fontId="167" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="168" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="82" fillId="0" fontId="169" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="170" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="83" fillId="0" fontId="171" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="172" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="84" fillId="0" fontId="173" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="174" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="85" fillId="0" fontId="175" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="176" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="86" fillId="0" fontId="177" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="178" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="87" fillId="0" fontId="179" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="180" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="88" fillId="0" fontId="181" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="182" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="89" fillId="0" fontId="183" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="184" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="90" fillId="0" fontId="185" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="186" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="91" fillId="0" fontId="187" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="188" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="92" fillId="0" fontId="189" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="190" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="93" fillId="0" fontId="191" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="192" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="94" fillId="0" fontId="193" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="194" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="95" fillId="0" fontId="195" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="196" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="96" fillId="0" fontId="197" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="198" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="97" fillId="0" fontId="199" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="200" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="98" fillId="0" fontId="201" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="202" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="99" fillId="0" fontId="203" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="204" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="100" fillId="0" fontId="205" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="206" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="101" fillId="0" fontId="207" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="208" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="102" fillId="0" fontId="209" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="210" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="103" fillId="0" fontId="211" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="212" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="104" fillId="0" fontId="213" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="214" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="105" fillId="0" fontId="215" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="216" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="106" fillId="0" fontId="217" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="218" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="107" fillId="0" fontId="219" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="220" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="108" fillId="0" fontId="221" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="222" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="109" fillId="0" fontId="223" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="224" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="110" fillId="0" fontId="225" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="226" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="111" fillId="0" fontId="227" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="228" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="112" fillId="0" fontId="229" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="230" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="113" fillId="0" fontId="231" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="232" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="114" fillId="0" fontId="233" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="234" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="115" fillId="0" fontId="235" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="236" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="116" fillId="0" fontId="237" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="238" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="117" fillId="0" fontId="239" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="240" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="118" fillId="0" fontId="241" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="242" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="119" fillId="0" fontId="243" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="244" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="120" fillId="0" fontId="245" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="246" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="121" fillId="0" fontId="247" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="248" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="122" fillId="0" fontId="249" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="250" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="123" fillId="0" fontId="251" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="252" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="124" fillId="0" fontId="253" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="254" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="125" fillId="0" fontId="255" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="256" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="126" fillId="0" fontId="257" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="258" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="127" fillId="0" fontId="259" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="260" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="128" fillId="0" fontId="261" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="262" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="129" fillId="0" fontId="263" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="264" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="130" fillId="0" fontId="265" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="266" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="131" fillId="0" fontId="267" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="268" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="132" fillId="0" fontId="269" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="270" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="133" fillId="0" fontId="271" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="272" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="134" fillId="0" fontId="273" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="274" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="135" fillId="0" fontId="275" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="276" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="136" fillId="0" fontId="277" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="278" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="137" fillId="0" fontId="279" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="280" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="138" fillId="0" fontId="281" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="282" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="139" fillId="0" fontId="283" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="284" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="140" fillId="0" fontId="285" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="286" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="141" fillId="0" fontId="287" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="288" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="142" fillId="0" fontId="289" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="290" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="143" fillId="0" fontId="291" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="292" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="144" fillId="0" fontId="293" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="294" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="145" fillId="0" fontId="295" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="296" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="146" fillId="0" fontId="297" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="298" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="147" fillId="0" fontId="299" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="300" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="148" fillId="0" fontId="301" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="302" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="149" fillId="0" fontId="303" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="304" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="150" fillId="0" fontId="305" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="306" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="151" fillId="0" fontId="307" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="308" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="152" fillId="0" fontId="309" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="310" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="153" fillId="0" fontId="311" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="312" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="154" fillId="0" fontId="313" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="314" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="155" fillId="0" fontId="315" numFmtId="49" xfId="0"/>
+    <xf numFmtId="164" fontId="316" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="317" fillId="0" borderId="156" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>

</xml_diff>